<commit_message>
Upload validation and error handling (#6327)
</commit_message>
<xml_diff>
--- a/spec/support/coDuplicateDates.xlsx
+++ b/spec/support/coDuplicateDates.xlsx
@@ -7,13 +7,13 @@
   <sheets>
     <sheet name="RO Non-Availability Dates" sheetId="1" r:id="rId4"/>
     <sheet name="Board Non-Availability Dates" sheetId="2" r:id="rId5"/>
-    <sheet name="RO &amp; CO Hearing Allocation" sheetId="3" r:id="rId6"/>
+    <sheet name="RO Allocations" sheetId="3" r:id="rId6"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="125">
   <si>
     <t>Example</t>
   </si>
@@ -381,13 +381,10 @@
     <t>Board Non-Availability Dates and Holidays in Date Range</t>
   </si>
   <si>
-    <t>Allocation of Regional Office Video Hearings and Central Office Hearings</t>
+    <t>Allocation of Regional Office Video Hearings</t>
   </si>
   <si>
     <t>Number of Hearing Days Allocated in Date Range</t>
-  </si>
-  <si>
-    <t>Central Office</t>
   </si>
   <si>
     <t xml:space="preserve">Des Moines, IA </t>
@@ -532,7 +529,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="40">
+  <borders count="36">
     <border>
       <left/>
       <right/>
@@ -881,34 +878,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right>
-        <color indexed="8"/>
-      </right>
-      <top style="thin">
-        <color indexed="12"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="8"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left>
-        <color indexed="8"/>
-      </left>
-      <right style="thin">
-        <color indexed="12"/>
-      </right>
-      <top style="thin">
-        <color indexed="12"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="12"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color indexed="8"/>
       </left>
@@ -939,49 +908,6 @@
         <color indexed="12"/>
       </left>
       <right style="thin">
-        <color indexed="12"/>
-      </right>
-      <top style="thin">
-        <color indexed="8"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="8"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="12"/>
-      </left>
-      <right style="thin">
-        <color indexed="8"/>
-      </right>
-      <top style="thin">
-        <color indexed="8"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="8"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="12"/>
-      </left>
-      <right style="thin">
-        <color indexed="8"/>
-      </right>
-      <top style="thin">
-        <color indexed="8"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="12"/>
-      </left>
-      <right style="thin">
         <color indexed="8"/>
       </right>
       <top style="thin">
@@ -999,7 +925,9 @@
       <right style="thin">
         <color indexed="8"/>
       </right>
-      <top/>
+      <top style="thin">
+        <color indexed="8"/>
+      </top>
       <bottom/>
       <diagonal/>
     </border>
@@ -1026,6 +954,17 @@
         <color indexed="8"/>
       </right>
       <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="12"/>
+      </left>
+      <right style="thin">
+        <color indexed="8"/>
+      </right>
+      <top/>
       <bottom style="thin">
         <color indexed="12"/>
       </bottom>
@@ -1037,7 +976,7 @@
       <alignment vertical="bottom"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="78">
+  <cellXfs count="73">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
@@ -1095,10 +1034,10 @@
     <xf numFmtId="14" fontId="8" fillId="5" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="right" vertical="bottom"/>
     </xf>
-    <xf numFmtId="59" fontId="0" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="59" fontId="0" fillId="5" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="59" fontId="0" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="59" fontId="0" fillId="5" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -1107,10 +1046,10 @@
     <xf numFmtId="14" fontId="8" fillId="4" borderId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="right" vertical="bottom"/>
     </xf>
-    <xf numFmtId="59" fontId="0" borderId="12" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="59" fontId="0" fillId="5" borderId="12" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="59" fontId="0" borderId="13" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="59" fontId="0" fillId="5" borderId="13" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="14" fontId="8" fillId="5" borderId="11" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -1122,13 +1061,13 @@
     <xf numFmtId="14" fontId="8" fillId="5" borderId="5" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="14" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="14" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="15" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="15" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="13" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="13" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="16" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -1137,19 +1076,19 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="17" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="59" fontId="0" borderId="18" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="59" fontId="0" fillId="5" borderId="18" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="19" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="19" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="20" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="20" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="21" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="59" fontId="0" borderId="22" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="59" fontId="0" fillId="5" borderId="22" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="23" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -1158,10 +1097,10 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="24" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="25" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="25" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="26" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="26" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
@@ -1173,7 +1112,7 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="12" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="12" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -1188,7 +1127,7 @@
     <xf numFmtId="14" fontId="13" fillId="5" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="10" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
@@ -1200,10 +1139,7 @@
     <xf numFmtId="0" fontId="14" fillId="2" borderId="28" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="29" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="30" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="18" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="5" borderId="13" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -1221,55 +1157,43 @@
     <xf numFmtId="49" fontId="7" fillId="4" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="12" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="4" fillId="3" borderId="29" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="9" fillId="5" borderId="30" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="3" borderId="31" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="9" fillId="5" borderId="32" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="8" fillId="5" borderId="10" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="8" fillId="5" borderId="33" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="31" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="34" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="35" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="bottom"/>
+    <xf numFmtId="14" fontId="0" fillId="5" borderId="32" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="right" vertical="bottom"/>
     </xf>
     <xf numFmtId="49" fontId="7" fillId="8" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="9" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="36" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="5" borderId="37" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="right" vertical="bottom"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="5" borderId="12" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="38" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="33" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="5" borderId="37" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="14" fontId="0" fillId="5" borderId="34" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="right" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="5" borderId="34" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="37" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="34" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="12" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="39" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="35" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
   </cellXfs>
@@ -1450,9 +1374,9 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="20000" dir="5400000">
+            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="23000" dir="5400000">
               <a:srgbClr val="000000">
-                <a:alpha val="38000"/>
+                <a:alpha val="35000"/>
               </a:srgbClr>
             </a:outerShdw>
           </a:effectLst>
@@ -1532,7 +1456,7 @@
         </a:effectLst>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -1560,10 +1484,10 @@
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
-            <a:latin typeface="Calibri"/>
-            <a:ea typeface="Calibri"/>
-            <a:cs typeface="Calibri"/>
-            <a:sym typeface="Calibri"/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+            <a:sym typeface="Helvetica"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -1819,9 +1743,9 @@
           <a:round/>
         </a:ln>
         <a:effectLst>
-          <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="20000" dir="5400000">
+          <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="23000" dir="5400000">
             <a:srgbClr val="000000">
-              <a:alpha val="38000"/>
+              <a:alpha val="35000"/>
             </a:srgbClr>
           </a:outerShdw>
         </a:effectLst>
@@ -2109,7 +2033,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -2137,10 +2061,10 @@
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
-            <a:latin typeface="Calibri"/>
-            <a:ea typeface="Calibri"/>
-            <a:cs typeface="Calibri"/>
-            <a:sym typeface="Calibri"/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+            <a:sym typeface="Helvetica"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -6353,7 +6277,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:N100"/>
+  <dimension ref="A1:N99"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -6382,30 +6306,30 @@
       </c>
       <c r="B1" s="53"/>
       <c r="C1" s="53"/>
-      <c r="D1" s="54"/>
-      <c r="E1" s="55"/>
-      <c r="F1" s="56"/>
-      <c r="G1" s="56"/>
-      <c r="H1" s="56"/>
-      <c r="I1" s="56"/>
-      <c r="J1" s="56"/>
-      <c r="K1" s="56"/>
-      <c r="L1" s="56"/>
-      <c r="M1" s="56"/>
-      <c r="N1" s="56"/>
+      <c r="D1" s="53"/>
+      <c r="E1" s="54"/>
+      <c r="F1" s="55"/>
+      <c r="G1" s="55"/>
+      <c r="H1" s="55"/>
+      <c r="I1" s="55"/>
+      <c r="J1" s="55"/>
+      <c r="K1" s="55"/>
+      <c r="L1" s="55"/>
+      <c r="M1" s="55"/>
+      <c r="N1" s="55"/>
     </row>
     <row r="2" ht="47.1" customHeight="1">
-      <c r="A2" s="57"/>
-      <c r="B2" t="s" s="58">
+      <c r="A2" s="56"/>
+      <c r="B2" t="s" s="57">
         <v>61</v>
       </c>
-      <c r="C2" t="s" s="59">
+      <c r="C2" t="s" s="58">
         <v>2</v>
       </c>
-      <c r="D2" t="s" s="60">
+      <c r="D2" t="s" s="59">
         <v>123</v>
       </c>
-      <c r="E2" s="61"/>
+      <c r="E2" s="45"/>
       <c r="F2" s="30"/>
       <c r="G2" s="30"/>
       <c r="H2" s="30"/>
@@ -6417,19 +6341,19 @@
       <c r="N2" s="30"/>
     </row>
     <row r="3" ht="39" customHeight="1">
-      <c r="A3" t="s" s="62">
+      <c r="A3" t="s" s="60">
         <v>0</v>
       </c>
-      <c r="B3" t="s" s="63">
+      <c r="B3" t="s" s="61">
         <v>62</v>
       </c>
-      <c r="C3" t="s" s="64">
+      <c r="C3" t="s" s="62">
         <v>3</v>
       </c>
-      <c r="D3" s="65">
+      <c r="D3" s="63">
         <v>10</v>
       </c>
-      <c r="E3" s="61"/>
+      <c r="E3" s="45"/>
       <c r="F3" s="30"/>
       <c r="G3" s="30"/>
       <c r="H3" s="30"/>
@@ -6440,16 +6364,18 @@
       <c r="M3" s="30"/>
       <c r="N3" s="30"/>
     </row>
-    <row r="4" ht="30.95" customHeight="1">
-      <c r="A4" s="66"/>
-      <c r="B4" t="s" s="67">
-        <v>124</v>
-      </c>
-      <c r="C4" s="68"/>
-      <c r="D4" s="69">
-        <v>5</v>
-      </c>
-      <c r="E4" s="61"/>
+    <row r="4" ht="15.75" customHeight="1">
+      <c r="A4" s="64"/>
+      <c r="B4" t="s" s="65">
+        <v>63</v>
+      </c>
+      <c r="C4" t="s" s="66">
+        <v>4</v>
+      </c>
+      <c r="D4" s="67">
+        <v>4</v>
+      </c>
+      <c r="E4" s="45"/>
       <c r="F4" s="30"/>
       <c r="G4" s="30"/>
       <c r="H4" s="30"/>
@@ -6461,17 +6387,17 @@
       <c r="N4" s="30"/>
     </row>
     <row r="5" ht="15.75" customHeight="1">
-      <c r="A5" s="70"/>
-      <c r="B5" t="s" s="67">
-        <v>63</v>
-      </c>
-      <c r="C5" t="s" s="71">
-        <v>4</v>
-      </c>
-      <c r="D5" s="72">
-        <v>4</v>
-      </c>
-      <c r="E5" s="61"/>
+      <c r="A5" s="68"/>
+      <c r="B5" t="s" s="65">
+        <v>64</v>
+      </c>
+      <c r="C5" t="s" s="66">
+        <v>5</v>
+      </c>
+      <c r="D5" s="67">
+        <v>10</v>
+      </c>
+      <c r="E5" s="45"/>
       <c r="F5" s="30"/>
       <c r="G5" s="30"/>
       <c r="H5" s="30"/>
@@ -6483,17 +6409,17 @@
       <c r="N5" s="30"/>
     </row>
     <row r="6" ht="15.75" customHeight="1">
-      <c r="A6" s="70"/>
-      <c r="B6" t="s" s="67">
-        <v>64</v>
-      </c>
-      <c r="C6" t="s" s="71">
-        <v>5</v>
-      </c>
-      <c r="D6" s="72">
-        <v>10</v>
-      </c>
-      <c r="E6" s="61"/>
+      <c r="A6" s="69"/>
+      <c r="B6" t="s" s="65">
+        <v>65</v>
+      </c>
+      <c r="C6" t="s" s="66">
+        <v>6</v>
+      </c>
+      <c r="D6" s="67">
+        <v>11</v>
+      </c>
+      <c r="E6" s="45"/>
       <c r="F6" s="30"/>
       <c r="G6" s="30"/>
       <c r="H6" s="30"/>
@@ -6505,17 +6431,17 @@
       <c r="N6" s="30"/>
     </row>
     <row r="7" ht="15.75" customHeight="1">
-      <c r="A7" s="73"/>
-      <c r="B7" t="s" s="67">
-        <v>65</v>
-      </c>
-      <c r="C7" t="s" s="71">
-        <v>6</v>
-      </c>
-      <c r="D7" s="72">
-        <v>11</v>
-      </c>
-      <c r="E7" s="61"/>
+      <c r="A7" s="69"/>
+      <c r="B7" t="s" s="65">
+        <v>66</v>
+      </c>
+      <c r="C7" t="s" s="66">
+        <v>7</v>
+      </c>
+      <c r="D7" s="67">
+        <v>7</v>
+      </c>
+      <c r="E7" s="45"/>
       <c r="F7" s="30"/>
       <c r="G7" s="30"/>
       <c r="H7" s="30"/>
@@ -6527,17 +6453,17 @@
       <c r="N7" s="30"/>
     </row>
     <row r="8" ht="15.75" customHeight="1">
-      <c r="A8" s="73"/>
-      <c r="B8" t="s" s="67">
-        <v>66</v>
-      </c>
-      <c r="C8" t="s" s="71">
-        <v>7</v>
-      </c>
-      <c r="D8" s="72">
-        <v>7</v>
-      </c>
-      <c r="E8" s="61"/>
+      <c r="A8" s="70"/>
+      <c r="B8" t="s" s="65">
+        <v>67</v>
+      </c>
+      <c r="C8" t="s" s="66">
+        <v>8</v>
+      </c>
+      <c r="D8" s="67">
+        <v>4</v>
+      </c>
+      <c r="E8" s="45"/>
       <c r="F8" s="30"/>
       <c r="G8" s="30"/>
       <c r="H8" s="30"/>
@@ -6549,17 +6475,17 @@
       <c r="N8" s="30"/>
     </row>
     <row r="9" ht="15.75" customHeight="1">
-      <c r="A9" s="74"/>
-      <c r="B9" t="s" s="67">
-        <v>67</v>
-      </c>
-      <c r="C9" t="s" s="71">
-        <v>8</v>
-      </c>
-      <c r="D9" s="72">
-        <v>4</v>
-      </c>
-      <c r="E9" s="61"/>
+      <c r="A9" s="70"/>
+      <c r="B9" t="s" s="65">
+        <v>68</v>
+      </c>
+      <c r="C9" t="s" s="66">
+        <v>9</v>
+      </c>
+      <c r="D9" s="67">
+        <v>6</v>
+      </c>
+      <c r="E9" s="45"/>
       <c r="F9" s="30"/>
       <c r="G9" s="30"/>
       <c r="H9" s="30"/>
@@ -6571,17 +6497,17 @@
       <c r="N9" s="30"/>
     </row>
     <row r="10" ht="15.75" customHeight="1">
-      <c r="A10" s="74"/>
-      <c r="B10" t="s" s="67">
-        <v>68</v>
-      </c>
-      <c r="C10" t="s" s="71">
-        <v>9</v>
-      </c>
-      <c r="D10" s="72">
-        <v>6</v>
-      </c>
-      <c r="E10" s="61"/>
+      <c r="A10" s="70"/>
+      <c r="B10" t="s" s="65">
+        <v>69</v>
+      </c>
+      <c r="C10" t="s" s="66">
+        <v>10</v>
+      </c>
+      <c r="D10" s="67">
+        <v>3</v>
+      </c>
+      <c r="E10" s="45"/>
       <c r="F10" s="30"/>
       <c r="G10" s="30"/>
       <c r="H10" s="30"/>
@@ -6593,17 +6519,17 @@
       <c r="N10" s="30"/>
     </row>
     <row r="11" ht="15.75" customHeight="1">
-      <c r="A11" s="74"/>
-      <c r="B11" t="s" s="67">
-        <v>69</v>
-      </c>
-      <c r="C11" t="s" s="71">
-        <v>10</v>
-      </c>
-      <c r="D11" s="72">
-        <v>3</v>
-      </c>
-      <c r="E11" s="61"/>
+      <c r="A11" s="70"/>
+      <c r="B11" t="s" s="65">
+        <v>70</v>
+      </c>
+      <c r="C11" t="s" s="66">
+        <v>11</v>
+      </c>
+      <c r="D11" s="67">
+        <v>1</v>
+      </c>
+      <c r="E11" s="45"/>
       <c r="F11" s="30"/>
       <c r="G11" s="30"/>
       <c r="H11" s="30"/>
@@ -6615,17 +6541,17 @@
       <c r="N11" s="30"/>
     </row>
     <row r="12" ht="15.75" customHeight="1">
-      <c r="A12" s="74"/>
-      <c r="B12" t="s" s="67">
-        <v>70</v>
-      </c>
-      <c r="C12" t="s" s="71">
-        <v>11</v>
-      </c>
-      <c r="D12" s="72">
-        <v>1</v>
-      </c>
-      <c r="E12" s="61"/>
+      <c r="A12" s="70"/>
+      <c r="B12" t="s" s="65">
+        <v>71</v>
+      </c>
+      <c r="C12" t="s" s="66">
+        <v>12</v>
+      </c>
+      <c r="D12" s="67">
+        <v>6</v>
+      </c>
+      <c r="E12" s="45"/>
       <c r="F12" s="30"/>
       <c r="G12" s="30"/>
       <c r="H12" s="30"/>
@@ -6637,17 +6563,17 @@
       <c r="N12" s="30"/>
     </row>
     <row r="13" ht="15.75" customHeight="1">
-      <c r="A13" s="74"/>
-      <c r="B13" t="s" s="67">
-        <v>71</v>
-      </c>
-      <c r="C13" t="s" s="71">
-        <v>12</v>
-      </c>
-      <c r="D13" s="72">
-        <v>6</v>
-      </c>
-      <c r="E13" s="61"/>
+      <c r="A13" s="70"/>
+      <c r="B13" t="s" s="65">
+        <v>72</v>
+      </c>
+      <c r="C13" t="s" s="66">
+        <v>13</v>
+      </c>
+      <c r="D13" s="67">
+        <v>8</v>
+      </c>
+      <c r="E13" s="45"/>
       <c r="F13" s="30"/>
       <c r="G13" s="30"/>
       <c r="H13" s="30"/>
@@ -6659,17 +6585,17 @@
       <c r="N13" s="30"/>
     </row>
     <row r="14" ht="15.75" customHeight="1">
-      <c r="A14" s="74"/>
-      <c r="B14" t="s" s="67">
-        <v>72</v>
-      </c>
-      <c r="C14" t="s" s="71">
-        <v>13</v>
-      </c>
-      <c r="D14" s="72">
-        <v>8</v>
-      </c>
-      <c r="E14" s="61"/>
+      <c r="A14" s="70"/>
+      <c r="B14" t="s" s="65">
+        <v>73</v>
+      </c>
+      <c r="C14" t="s" s="66">
+        <v>14</v>
+      </c>
+      <c r="D14" s="67">
+        <v>9</v>
+      </c>
+      <c r="E14" s="45"/>
       <c r="F14" s="30"/>
       <c r="G14" s="30"/>
       <c r="H14" s="30"/>
@@ -6681,17 +6607,17 @@
       <c r="N14" s="30"/>
     </row>
     <row r="15" ht="15.75" customHeight="1">
-      <c r="A15" s="74"/>
-      <c r="B15" t="s" s="67">
-        <v>73</v>
-      </c>
-      <c r="C15" t="s" s="71">
-        <v>14</v>
-      </c>
-      <c r="D15" s="72">
-        <v>9</v>
-      </c>
-      <c r="E15" s="61"/>
+      <c r="A15" s="70"/>
+      <c r="B15" t="s" s="65">
+        <v>74</v>
+      </c>
+      <c r="C15" t="s" s="66">
+        <v>15</v>
+      </c>
+      <c r="D15" s="67">
+        <v>5</v>
+      </c>
+      <c r="E15" s="45"/>
       <c r="F15" s="30"/>
       <c r="G15" s="30"/>
       <c r="H15" s="30"/>
@@ -6703,17 +6629,17 @@
       <c r="N15" s="30"/>
     </row>
     <row r="16" ht="15.75" customHeight="1">
-      <c r="A16" s="74"/>
-      <c r="B16" t="s" s="67">
-        <v>74</v>
-      </c>
-      <c r="C16" t="s" s="71">
-        <v>15</v>
-      </c>
-      <c r="D16" s="72">
-        <v>5</v>
-      </c>
-      <c r="E16" s="61"/>
+      <c r="A16" s="70"/>
+      <c r="B16" t="s" s="65">
+        <v>75</v>
+      </c>
+      <c r="C16" t="s" s="66">
+        <v>16</v>
+      </c>
+      <c r="D16" s="67">
+        <v>4</v>
+      </c>
+      <c r="E16" s="45"/>
       <c r="F16" s="30"/>
       <c r="G16" s="30"/>
       <c r="H16" s="30"/>
@@ -6725,17 +6651,17 @@
       <c r="N16" s="30"/>
     </row>
     <row r="17" ht="15.75" customHeight="1">
-      <c r="A17" s="74"/>
-      <c r="B17" t="s" s="67">
-        <v>75</v>
-      </c>
-      <c r="C17" t="s" s="71">
-        <v>16</v>
-      </c>
-      <c r="D17" s="72">
-        <v>4</v>
-      </c>
-      <c r="E17" s="61"/>
+      <c r="A17" s="70"/>
+      <c r="B17" t="s" s="65">
+        <v>76</v>
+      </c>
+      <c r="C17" t="s" s="66">
+        <v>17</v>
+      </c>
+      <c r="D17" s="67">
+        <v>2</v>
+      </c>
+      <c r="E17" s="45"/>
       <c r="F17" s="30"/>
       <c r="G17" s="30"/>
       <c r="H17" s="30"/>
@@ -6747,17 +6673,17 @@
       <c r="N17" s="30"/>
     </row>
     <row r="18" ht="15.75" customHeight="1">
-      <c r="A18" s="74"/>
-      <c r="B18" t="s" s="67">
-        <v>76</v>
-      </c>
-      <c r="C18" t="s" s="71">
-        <v>17</v>
-      </c>
-      <c r="D18" s="72">
-        <v>2</v>
-      </c>
-      <c r="E18" s="61"/>
+      <c r="A18" s="70"/>
+      <c r="B18" t="s" s="65">
+        <v>77</v>
+      </c>
+      <c r="C18" t="s" s="66">
+        <v>18</v>
+      </c>
+      <c r="D18" s="67">
+        <v>5</v>
+      </c>
+      <c r="E18" s="45"/>
       <c r="F18" s="30"/>
       <c r="G18" s="30"/>
       <c r="H18" s="30"/>
@@ -6769,17 +6695,17 @@
       <c r="N18" s="30"/>
     </row>
     <row r="19" ht="15.75" customHeight="1">
-      <c r="A19" s="74"/>
-      <c r="B19" t="s" s="67">
-        <v>77</v>
-      </c>
-      <c r="C19" t="s" s="71">
-        <v>18</v>
-      </c>
-      <c r="D19" s="72">
-        <v>5</v>
-      </c>
-      <c r="E19" s="61"/>
+      <c r="A19" s="70"/>
+      <c r="B19" t="s" s="65">
+        <v>78</v>
+      </c>
+      <c r="C19" t="s" s="66">
+        <v>19</v>
+      </c>
+      <c r="D19" s="67">
+        <v>7</v>
+      </c>
+      <c r="E19" s="45"/>
       <c r="F19" s="30"/>
       <c r="G19" s="30"/>
       <c r="H19" s="30"/>
@@ -6791,17 +6717,17 @@
       <c r="N19" s="30"/>
     </row>
     <row r="20" ht="15.75" customHeight="1">
-      <c r="A20" s="74"/>
-      <c r="B20" t="s" s="67">
-        <v>78</v>
-      </c>
-      <c r="C20" t="s" s="71">
-        <v>19</v>
-      </c>
-      <c r="D20" s="72">
-        <v>7</v>
-      </c>
-      <c r="E20" s="61"/>
+      <c r="A20" s="70"/>
+      <c r="B20" t="s" s="65">
+        <v>79</v>
+      </c>
+      <c r="C20" t="s" s="66">
+        <v>20</v>
+      </c>
+      <c r="D20" s="67">
+        <v>15</v>
+      </c>
+      <c r="E20" s="45"/>
       <c r="F20" s="30"/>
       <c r="G20" s="30"/>
       <c r="H20" s="30"/>
@@ -6813,17 +6739,17 @@
       <c r="N20" s="30"/>
     </row>
     <row r="21" ht="15.75" customHeight="1">
-      <c r="A21" s="74"/>
-      <c r="B21" t="s" s="67">
-        <v>79</v>
-      </c>
-      <c r="C21" t="s" s="71">
-        <v>20</v>
-      </c>
-      <c r="D21" s="72">
-        <v>15</v>
-      </c>
-      <c r="E21" s="61"/>
+      <c r="A21" s="70"/>
+      <c r="B21" t="s" s="65">
+        <v>80</v>
+      </c>
+      <c r="C21" t="s" s="66">
+        <v>21</v>
+      </c>
+      <c r="D21" s="67">
+        <v>3</v>
+      </c>
+      <c r="E21" s="45"/>
       <c r="F21" s="30"/>
       <c r="G21" s="30"/>
       <c r="H21" s="30"/>
@@ -6835,17 +6761,17 @@
       <c r="N21" s="30"/>
     </row>
     <row r="22" ht="15.75" customHeight="1">
-      <c r="A22" s="74"/>
-      <c r="B22" t="s" s="67">
-        <v>80</v>
-      </c>
-      <c r="C22" t="s" s="71">
-        <v>21</v>
-      </c>
-      <c r="D22" s="72">
-        <v>3</v>
-      </c>
-      <c r="E22" s="61"/>
+      <c r="A22" s="70"/>
+      <c r="B22" t="s" s="65">
+        <v>81</v>
+      </c>
+      <c r="C22" t="s" s="66">
+        <v>22</v>
+      </c>
+      <c r="D22" s="67">
+        <v>7</v>
+      </c>
+      <c r="E22" s="45"/>
       <c r="F22" s="30"/>
       <c r="G22" s="30"/>
       <c r="H22" s="30"/>
@@ -6857,17 +6783,17 @@
       <c r="N22" s="30"/>
     </row>
     <row r="23" ht="15.75" customHeight="1">
-      <c r="A23" s="74"/>
-      <c r="B23" t="s" s="67">
-        <v>81</v>
-      </c>
-      <c r="C23" t="s" s="71">
-        <v>22</v>
-      </c>
-      <c r="D23" s="72">
-        <v>7</v>
-      </c>
-      <c r="E23" s="61"/>
+      <c r="A23" s="70"/>
+      <c r="B23" t="s" s="65">
+        <v>82</v>
+      </c>
+      <c r="C23" t="s" s="66">
+        <v>23</v>
+      </c>
+      <c r="D23" s="67">
+        <v>0</v>
+      </c>
+      <c r="E23" s="45"/>
       <c r="F23" s="30"/>
       <c r="G23" s="30"/>
       <c r="H23" s="30"/>
@@ -6879,17 +6805,17 @@
       <c r="N23" s="30"/>
     </row>
     <row r="24" ht="15.75" customHeight="1">
-      <c r="A24" s="74"/>
-      <c r="B24" t="s" s="67">
-        <v>82</v>
-      </c>
-      <c r="C24" t="s" s="71">
-        <v>23</v>
-      </c>
-      <c r="D24" s="72">
-        <v>0</v>
-      </c>
-      <c r="E24" s="61"/>
+      <c r="A24" s="70"/>
+      <c r="B24" t="s" s="65">
+        <v>83</v>
+      </c>
+      <c r="C24" t="s" s="66">
+        <v>24</v>
+      </c>
+      <c r="D24" s="67">
+        <v>3</v>
+      </c>
+      <c r="E24" s="45"/>
       <c r="F24" s="30"/>
       <c r="G24" s="30"/>
       <c r="H24" s="30"/>
@@ -6901,17 +6827,17 @@
       <c r="N24" s="30"/>
     </row>
     <row r="25" ht="15.75" customHeight="1">
-      <c r="A25" s="74"/>
-      <c r="B25" t="s" s="67">
-        <v>83</v>
-      </c>
-      <c r="C25" t="s" s="71">
-        <v>24</v>
-      </c>
-      <c r="D25" s="72">
-        <v>3</v>
-      </c>
-      <c r="E25" s="61"/>
+      <c r="A25" s="70"/>
+      <c r="B25" t="s" s="65">
+        <v>84</v>
+      </c>
+      <c r="C25" t="s" s="66">
+        <v>25</v>
+      </c>
+      <c r="D25" s="67">
+        <v>7</v>
+      </c>
+      <c r="E25" s="45"/>
       <c r="F25" s="30"/>
       <c r="G25" s="30"/>
       <c r="H25" s="30"/>
@@ -6923,17 +6849,17 @@
       <c r="N25" s="30"/>
     </row>
     <row r="26" ht="15.75" customHeight="1">
-      <c r="A26" s="74"/>
-      <c r="B26" t="s" s="67">
-        <v>84</v>
-      </c>
-      <c r="C26" t="s" s="71">
-        <v>25</v>
-      </c>
-      <c r="D26" s="72">
-        <v>7</v>
-      </c>
-      <c r="E26" s="61"/>
+      <c r="A26" s="70"/>
+      <c r="B26" t="s" s="65">
+        <v>85</v>
+      </c>
+      <c r="C26" t="s" s="66">
+        <v>26</v>
+      </c>
+      <c r="D26" s="67">
+        <v>3</v>
+      </c>
+      <c r="E26" s="45"/>
       <c r="F26" s="30"/>
       <c r="G26" s="30"/>
       <c r="H26" s="30"/>
@@ -6945,17 +6871,17 @@
       <c r="N26" s="30"/>
     </row>
     <row r="27" ht="15.75" customHeight="1">
-      <c r="A27" s="74"/>
-      <c r="B27" t="s" s="67">
-        <v>85</v>
-      </c>
-      <c r="C27" t="s" s="71">
-        <v>26</v>
-      </c>
-      <c r="D27" s="72">
-        <v>3</v>
-      </c>
-      <c r="E27" s="61"/>
+      <c r="A27" s="70"/>
+      <c r="B27" t="s" s="65">
+        <v>86</v>
+      </c>
+      <c r="C27" t="s" s="66">
+        <v>27</v>
+      </c>
+      <c r="D27" s="67">
+        <v>2</v>
+      </c>
+      <c r="E27" s="45"/>
       <c r="F27" s="30"/>
       <c r="G27" s="30"/>
       <c r="H27" s="30"/>
@@ -6967,17 +6893,17 @@
       <c r="N27" s="30"/>
     </row>
     <row r="28" ht="15.75" customHeight="1">
-      <c r="A28" s="74"/>
-      <c r="B28" t="s" s="67">
-        <v>86</v>
-      </c>
-      <c r="C28" t="s" s="71">
-        <v>27</v>
-      </c>
-      <c r="D28" s="72">
-        <v>2</v>
-      </c>
-      <c r="E28" s="61"/>
+      <c r="A28" s="70"/>
+      <c r="B28" t="s" s="65">
+        <v>87</v>
+      </c>
+      <c r="C28" t="s" s="66">
+        <v>28</v>
+      </c>
+      <c r="D28" s="67">
+        <v>5</v>
+      </c>
+      <c r="E28" s="45"/>
       <c r="F28" s="30"/>
       <c r="G28" s="30"/>
       <c r="H28" s="30"/>
@@ -6989,17 +6915,17 @@
       <c r="N28" s="30"/>
     </row>
     <row r="29" ht="15.75" customHeight="1">
-      <c r="A29" s="74"/>
-      <c r="B29" t="s" s="67">
-        <v>87</v>
-      </c>
-      <c r="C29" t="s" s="71">
-        <v>28</v>
-      </c>
-      <c r="D29" s="72">
-        <v>5</v>
-      </c>
-      <c r="E29" s="61"/>
+      <c r="A29" s="70"/>
+      <c r="B29" t="s" s="65">
+        <v>88</v>
+      </c>
+      <c r="C29" t="s" s="66">
+        <v>29</v>
+      </c>
+      <c r="D29" s="67">
+        <v>7</v>
+      </c>
+      <c r="E29" s="45"/>
       <c r="F29" s="30"/>
       <c r="G29" s="30"/>
       <c r="H29" s="30"/>
@@ -7011,17 +6937,17 @@
       <c r="N29" s="30"/>
     </row>
     <row r="30" ht="15.75" customHeight="1">
-      <c r="A30" s="74"/>
-      <c r="B30" t="s" s="67">
-        <v>88</v>
-      </c>
-      <c r="C30" t="s" s="71">
-        <v>29</v>
-      </c>
-      <c r="D30" s="72">
-        <v>7</v>
-      </c>
-      <c r="E30" s="61"/>
+      <c r="A30" s="70"/>
+      <c r="B30" t="s" s="65">
+        <v>89</v>
+      </c>
+      <c r="C30" t="s" s="66">
+        <v>30</v>
+      </c>
+      <c r="D30" s="67">
+        <v>4</v>
+      </c>
+      <c r="E30" s="45"/>
       <c r="F30" s="30"/>
       <c r="G30" s="30"/>
       <c r="H30" s="30"/>
@@ -7033,17 +6959,17 @@
       <c r="N30" s="30"/>
     </row>
     <row r="31" ht="15.75" customHeight="1">
-      <c r="A31" s="74"/>
-      <c r="B31" t="s" s="67">
-        <v>89</v>
-      </c>
-      <c r="C31" t="s" s="71">
-        <v>30</v>
-      </c>
-      <c r="D31" s="72">
+      <c r="A31" s="70"/>
+      <c r="B31" t="s" s="65">
+        <v>90</v>
+      </c>
+      <c r="C31" t="s" s="66">
+        <v>31</v>
+      </c>
+      <c r="D31" s="67">
         <v>4</v>
       </c>
-      <c r="E31" s="61"/>
+      <c r="E31" s="45"/>
       <c r="F31" s="30"/>
       <c r="G31" s="30"/>
       <c r="H31" s="30"/>
@@ -7055,17 +6981,17 @@
       <c r="N31" s="30"/>
     </row>
     <row r="32" ht="15.75" customHeight="1">
-      <c r="A32" s="74"/>
-      <c r="B32" t="s" s="67">
-        <v>90</v>
-      </c>
-      <c r="C32" t="s" s="71">
-        <v>31</v>
-      </c>
-      <c r="D32" s="72">
-        <v>4</v>
-      </c>
-      <c r="E32" s="61"/>
+      <c r="A32" s="70"/>
+      <c r="B32" t="s" s="65">
+        <v>124</v>
+      </c>
+      <c r="C32" t="s" s="66">
+        <v>32</v>
+      </c>
+      <c r="D32" s="67">
+        <v>2</v>
+      </c>
+      <c r="E32" s="45"/>
       <c r="F32" s="30"/>
       <c r="G32" s="30"/>
       <c r="H32" s="30"/>
@@ -7077,17 +7003,17 @@
       <c r="N32" s="30"/>
     </row>
     <row r="33" ht="15.75" customHeight="1">
-      <c r="A33" s="74"/>
-      <c r="B33" t="s" s="67">
-        <v>125</v>
-      </c>
-      <c r="C33" t="s" s="71">
-        <v>32</v>
-      </c>
-      <c r="D33" s="72">
-        <v>2</v>
-      </c>
-      <c r="E33" s="61"/>
+      <c r="A33" s="70"/>
+      <c r="B33" t="s" s="65">
+        <v>92</v>
+      </c>
+      <c r="C33" t="s" s="66">
+        <v>33</v>
+      </c>
+      <c r="D33" s="67">
+        <v>5</v>
+      </c>
+      <c r="E33" s="45"/>
       <c r="F33" s="30"/>
       <c r="G33" s="30"/>
       <c r="H33" s="30"/>
@@ -7099,17 +7025,17 @@
       <c r="N33" s="30"/>
     </row>
     <row r="34" ht="15.75" customHeight="1">
-      <c r="A34" s="74"/>
-      <c r="B34" t="s" s="67">
-        <v>92</v>
-      </c>
-      <c r="C34" t="s" s="71">
-        <v>33</v>
-      </c>
-      <c r="D34" s="72">
-        <v>5</v>
-      </c>
-      <c r="E34" s="61"/>
+      <c r="A34" s="70"/>
+      <c r="B34" t="s" s="65">
+        <v>93</v>
+      </c>
+      <c r="C34" t="s" s="66">
+        <v>34</v>
+      </c>
+      <c r="D34" s="67">
+        <v>7</v>
+      </c>
+      <c r="E34" s="45"/>
       <c r="F34" s="30"/>
       <c r="G34" s="30"/>
       <c r="H34" s="30"/>
@@ -7121,17 +7047,17 @@
       <c r="N34" s="30"/>
     </row>
     <row r="35" ht="15.75" customHeight="1">
-      <c r="A35" s="74"/>
-      <c r="B35" t="s" s="67">
-        <v>93</v>
-      </c>
-      <c r="C35" t="s" s="71">
-        <v>34</v>
-      </c>
-      <c r="D35" s="72">
-        <v>7</v>
-      </c>
-      <c r="E35" s="61"/>
+      <c r="A35" s="70"/>
+      <c r="B35" t="s" s="65">
+        <v>94</v>
+      </c>
+      <c r="C35" t="s" s="66">
+        <v>35</v>
+      </c>
+      <c r="D35" s="67">
+        <v>9</v>
+      </c>
+      <c r="E35" s="45"/>
       <c r="F35" s="30"/>
       <c r="G35" s="30"/>
       <c r="H35" s="30"/>
@@ -7143,17 +7069,17 @@
       <c r="N35" s="30"/>
     </row>
     <row r="36" ht="15.75" customHeight="1">
-      <c r="A36" s="74"/>
-      <c r="B36" t="s" s="67">
-        <v>94</v>
-      </c>
-      <c r="C36" t="s" s="71">
-        <v>35</v>
-      </c>
-      <c r="D36" s="72">
-        <v>9</v>
-      </c>
-      <c r="E36" s="61"/>
+      <c r="A36" s="70"/>
+      <c r="B36" t="s" s="65">
+        <v>95</v>
+      </c>
+      <c r="C36" t="s" s="66">
+        <v>36</v>
+      </c>
+      <c r="D36" s="67">
+        <v>4</v>
+      </c>
+      <c r="E36" s="45"/>
       <c r="F36" s="30"/>
       <c r="G36" s="30"/>
       <c r="H36" s="30"/>
@@ -7165,17 +7091,17 @@
       <c r="N36" s="30"/>
     </row>
     <row r="37" ht="15.75" customHeight="1">
-      <c r="A37" s="74"/>
-      <c r="B37" t="s" s="67">
-        <v>95</v>
-      </c>
-      <c r="C37" t="s" s="71">
-        <v>36</v>
-      </c>
-      <c r="D37" s="72">
-        <v>4</v>
-      </c>
-      <c r="E37" s="61"/>
+      <c r="A37" s="70"/>
+      <c r="B37" t="s" s="65">
+        <v>96</v>
+      </c>
+      <c r="C37" t="s" s="66">
+        <v>37</v>
+      </c>
+      <c r="D37" s="67">
+        <v>2</v>
+      </c>
+      <c r="E37" s="45"/>
       <c r="F37" s="30"/>
       <c r="G37" s="30"/>
       <c r="H37" s="30"/>
@@ -7187,17 +7113,17 @@
       <c r="N37" s="30"/>
     </row>
     <row r="38" ht="15.75" customHeight="1">
-      <c r="A38" s="74"/>
-      <c r="B38" t="s" s="67">
-        <v>96</v>
-      </c>
-      <c r="C38" t="s" s="71">
-        <v>37</v>
-      </c>
-      <c r="D38" s="72">
-        <v>2</v>
-      </c>
-      <c r="E38" s="61"/>
+      <c r="A38" s="70"/>
+      <c r="B38" t="s" s="65">
+        <v>97</v>
+      </c>
+      <c r="C38" t="s" s="66">
+        <v>38</v>
+      </c>
+      <c r="D38" s="67">
+        <v>6</v>
+      </c>
+      <c r="E38" s="45"/>
       <c r="F38" s="30"/>
       <c r="G38" s="30"/>
       <c r="H38" s="30"/>
@@ -7209,17 +7135,17 @@
       <c r="N38" s="30"/>
     </row>
     <row r="39" ht="15.75" customHeight="1">
-      <c r="A39" s="74"/>
-      <c r="B39" t="s" s="67">
-        <v>97</v>
-      </c>
-      <c r="C39" t="s" s="71">
-        <v>38</v>
-      </c>
-      <c r="D39" s="72">
-        <v>6</v>
-      </c>
-      <c r="E39" s="61"/>
+      <c r="A39" s="70"/>
+      <c r="B39" t="s" s="65">
+        <v>98</v>
+      </c>
+      <c r="C39" t="s" s="66">
+        <v>39</v>
+      </c>
+      <c r="D39" s="67">
+        <v>3</v>
+      </c>
+      <c r="E39" s="45"/>
       <c r="F39" s="30"/>
       <c r="G39" s="30"/>
       <c r="H39" s="30"/>
@@ -7231,17 +7157,17 @@
       <c r="N39" s="30"/>
     </row>
     <row r="40" ht="15.75" customHeight="1">
-      <c r="A40" s="74"/>
-      <c r="B40" t="s" s="67">
-        <v>98</v>
-      </c>
-      <c r="C40" t="s" s="71">
-        <v>39</v>
-      </c>
-      <c r="D40" s="72">
-        <v>3</v>
-      </c>
-      <c r="E40" s="61"/>
+      <c r="A40" s="70"/>
+      <c r="B40" t="s" s="65">
+        <v>99</v>
+      </c>
+      <c r="C40" t="s" s="66">
+        <v>40</v>
+      </c>
+      <c r="D40" s="67">
+        <v>2</v>
+      </c>
+      <c r="E40" s="45"/>
       <c r="F40" s="30"/>
       <c r="G40" s="30"/>
       <c r="H40" s="30"/>
@@ -7253,17 +7179,17 @@
       <c r="N40" s="30"/>
     </row>
     <row r="41" ht="15.75" customHeight="1">
-      <c r="A41" s="74"/>
-      <c r="B41" t="s" s="67">
-        <v>99</v>
-      </c>
-      <c r="C41" t="s" s="71">
-        <v>40</v>
-      </c>
-      <c r="D41" s="72">
-        <v>2</v>
-      </c>
-      <c r="E41" s="61"/>
+      <c r="A41" s="70"/>
+      <c r="B41" t="s" s="65">
+        <v>100</v>
+      </c>
+      <c r="C41" t="s" s="66">
+        <v>41</v>
+      </c>
+      <c r="D41" s="67">
+        <v>6</v>
+      </c>
+      <c r="E41" s="45"/>
       <c r="F41" s="30"/>
       <c r="G41" s="30"/>
       <c r="H41" s="30"/>
@@ -7275,17 +7201,17 @@
       <c r="N41" s="30"/>
     </row>
     <row r="42" ht="15.75" customHeight="1">
-      <c r="A42" s="74"/>
-      <c r="B42" t="s" s="67">
-        <v>100</v>
-      </c>
-      <c r="C42" t="s" s="71">
-        <v>41</v>
-      </c>
-      <c r="D42" s="72">
-        <v>6</v>
-      </c>
-      <c r="E42" s="61"/>
+      <c r="A42" s="70"/>
+      <c r="B42" t="s" s="65">
+        <v>101</v>
+      </c>
+      <c r="C42" t="s" s="66">
+        <v>42</v>
+      </c>
+      <c r="D42" s="67">
+        <v>5</v>
+      </c>
+      <c r="E42" s="45"/>
       <c r="F42" s="30"/>
       <c r="G42" s="30"/>
       <c r="H42" s="30"/>
@@ -7297,17 +7223,17 @@
       <c r="N42" s="30"/>
     </row>
     <row r="43" ht="15.75" customHeight="1">
-      <c r="A43" s="74"/>
-      <c r="B43" t="s" s="67">
-        <v>101</v>
-      </c>
-      <c r="C43" t="s" s="71">
-        <v>42</v>
-      </c>
-      <c r="D43" s="72">
-        <v>5</v>
-      </c>
-      <c r="E43" s="61"/>
+      <c r="A43" s="70"/>
+      <c r="B43" t="s" s="65">
+        <v>102</v>
+      </c>
+      <c r="C43" t="s" s="66">
+        <v>43</v>
+      </c>
+      <c r="D43" s="67">
+        <v>3</v>
+      </c>
+      <c r="E43" s="45"/>
       <c r="F43" s="30"/>
       <c r="G43" s="30"/>
       <c r="H43" s="30"/>
@@ -7319,17 +7245,17 @@
       <c r="N43" s="30"/>
     </row>
     <row r="44" ht="15.75" customHeight="1">
-      <c r="A44" s="74"/>
-      <c r="B44" t="s" s="67">
-        <v>102</v>
-      </c>
-      <c r="C44" t="s" s="71">
-        <v>43</v>
-      </c>
-      <c r="D44" s="72">
-        <v>3</v>
-      </c>
-      <c r="E44" s="61"/>
+      <c r="A44" s="70"/>
+      <c r="B44" t="s" s="65">
+        <v>103</v>
+      </c>
+      <c r="C44" t="s" s="66">
+        <v>44</v>
+      </c>
+      <c r="D44" s="67">
+        <v>5</v>
+      </c>
+      <c r="E44" s="45"/>
       <c r="F44" s="30"/>
       <c r="G44" s="30"/>
       <c r="H44" s="30"/>
@@ -7341,17 +7267,17 @@
       <c r="N44" s="30"/>
     </row>
     <row r="45" ht="15.75" customHeight="1">
-      <c r="A45" s="74"/>
-      <c r="B45" t="s" s="67">
-        <v>103</v>
-      </c>
-      <c r="C45" t="s" s="71">
-        <v>44</v>
-      </c>
-      <c r="D45" s="72">
-        <v>5</v>
-      </c>
-      <c r="E45" s="61"/>
+      <c r="A45" s="70"/>
+      <c r="B45" t="s" s="65">
+        <v>104</v>
+      </c>
+      <c r="C45" t="s" s="66">
+        <v>45</v>
+      </c>
+      <c r="D45" s="67">
+        <v>36</v>
+      </c>
+      <c r="E45" s="45"/>
       <c r="F45" s="30"/>
       <c r="G45" s="30"/>
       <c r="H45" s="30"/>
@@ -7363,17 +7289,17 @@
       <c r="N45" s="30"/>
     </row>
     <row r="46" ht="15.75" customHeight="1">
-      <c r="A46" s="74"/>
-      <c r="B46" t="s" s="67">
-        <v>104</v>
-      </c>
-      <c r="C46" t="s" s="71">
-        <v>45</v>
-      </c>
-      <c r="D46" s="72">
-        <v>36</v>
-      </c>
-      <c r="E46" s="61"/>
+      <c r="A46" s="70"/>
+      <c r="B46" t="s" s="65">
+        <v>105</v>
+      </c>
+      <c r="C46" t="s" s="66">
+        <v>46</v>
+      </c>
+      <c r="D46" s="67">
+        <v>7</v>
+      </c>
+      <c r="E46" s="45"/>
       <c r="F46" s="30"/>
       <c r="G46" s="30"/>
       <c r="H46" s="30"/>
@@ -7385,17 +7311,17 @@
       <c r="N46" s="30"/>
     </row>
     <row r="47" ht="15.75" customHeight="1">
-      <c r="A47" s="74"/>
-      <c r="B47" t="s" s="67">
-        <v>105</v>
-      </c>
-      <c r="C47" t="s" s="71">
-        <v>46</v>
-      </c>
-      <c r="D47" s="72">
-        <v>7</v>
-      </c>
-      <c r="E47" s="61"/>
+      <c r="A47" s="70"/>
+      <c r="B47" t="s" s="65">
+        <v>106</v>
+      </c>
+      <c r="C47" t="s" s="66">
+        <v>47</v>
+      </c>
+      <c r="D47" s="67">
+        <v>1</v>
+      </c>
+      <c r="E47" s="45"/>
       <c r="F47" s="30"/>
       <c r="G47" s="30"/>
       <c r="H47" s="30"/>
@@ -7407,17 +7333,17 @@
       <c r="N47" s="30"/>
     </row>
     <row r="48" ht="15.75" customHeight="1">
-      <c r="A48" s="74"/>
-      <c r="B48" t="s" s="67">
-        <v>106</v>
-      </c>
-      <c r="C48" t="s" s="71">
-        <v>47</v>
-      </c>
-      <c r="D48" s="72">
-        <v>1</v>
-      </c>
-      <c r="E48" s="61"/>
+      <c r="A48" s="70"/>
+      <c r="B48" t="s" s="65">
+        <v>107</v>
+      </c>
+      <c r="C48" t="s" s="66">
+        <v>48</v>
+      </c>
+      <c r="D48" s="67">
+        <v>4</v>
+      </c>
+      <c r="E48" s="45"/>
       <c r="F48" s="30"/>
       <c r="G48" s="30"/>
       <c r="H48" s="30"/>
@@ -7429,17 +7355,17 @@
       <c r="N48" s="30"/>
     </row>
     <row r="49" ht="15.75" customHeight="1">
-      <c r="A49" s="74"/>
-      <c r="B49" t="s" s="67">
-        <v>107</v>
-      </c>
-      <c r="C49" t="s" s="71">
-        <v>48</v>
-      </c>
-      <c r="D49" s="72">
-        <v>4</v>
-      </c>
-      <c r="E49" s="61"/>
+      <c r="A49" s="70"/>
+      <c r="B49" t="s" s="65">
+        <v>108</v>
+      </c>
+      <c r="C49" t="s" s="66">
+        <v>49</v>
+      </c>
+      <c r="D49" s="67">
+        <v>57</v>
+      </c>
+      <c r="E49" s="45"/>
       <c r="F49" s="30"/>
       <c r="G49" s="30"/>
       <c r="H49" s="30"/>
@@ -7451,17 +7377,17 @@
       <c r="N49" s="30"/>
     </row>
     <row r="50" ht="15.75" customHeight="1">
-      <c r="A50" s="74"/>
-      <c r="B50" t="s" s="67">
-        <v>108</v>
-      </c>
-      <c r="C50" t="s" s="71">
-        <v>49</v>
-      </c>
-      <c r="D50" s="72">
-        <v>57</v>
-      </c>
-      <c r="E50" s="61"/>
+      <c r="A50" s="70"/>
+      <c r="B50" t="s" s="65">
+        <v>109</v>
+      </c>
+      <c r="C50" t="s" s="66">
+        <v>50</v>
+      </c>
+      <c r="D50" s="67">
+        <v>3</v>
+      </c>
+      <c r="E50" s="45"/>
       <c r="F50" s="30"/>
       <c r="G50" s="30"/>
       <c r="H50" s="30"/>
@@ -7473,17 +7399,17 @@
       <c r="N50" s="30"/>
     </row>
     <row r="51" ht="15.75" customHeight="1">
-      <c r="A51" s="74"/>
-      <c r="B51" t="s" s="67">
-        <v>109</v>
-      </c>
-      <c r="C51" t="s" s="71">
-        <v>50</v>
-      </c>
-      <c r="D51" s="72">
-        <v>3</v>
-      </c>
-      <c r="E51" s="61"/>
+      <c r="A51" s="70"/>
+      <c r="B51" t="s" s="65">
+        <v>110</v>
+      </c>
+      <c r="C51" t="s" s="66">
+        <v>51</v>
+      </c>
+      <c r="D51" s="67">
+        <v>1</v>
+      </c>
+      <c r="E51" s="45"/>
       <c r="F51" s="30"/>
       <c r="G51" s="30"/>
       <c r="H51" s="30"/>
@@ -7495,17 +7421,17 @@
       <c r="N51" s="30"/>
     </row>
     <row r="52" ht="15.75" customHeight="1">
-      <c r="A52" s="74"/>
-      <c r="B52" t="s" s="67">
-        <v>110</v>
-      </c>
-      <c r="C52" t="s" s="71">
-        <v>51</v>
-      </c>
-      <c r="D52" s="72">
-        <v>1</v>
-      </c>
-      <c r="E52" s="61"/>
+      <c r="A52" s="70"/>
+      <c r="B52" t="s" s="65">
+        <v>111</v>
+      </c>
+      <c r="C52" t="s" s="66">
+        <v>52</v>
+      </c>
+      <c r="D52" s="67">
+        <v>7</v>
+      </c>
+      <c r="E52" s="45"/>
       <c r="F52" s="30"/>
       <c r="G52" s="30"/>
       <c r="H52" s="30"/>
@@ -7517,17 +7443,17 @@
       <c r="N52" s="30"/>
     </row>
     <row r="53" ht="15.75" customHeight="1">
-      <c r="A53" s="74"/>
-      <c r="B53" t="s" s="67">
-        <v>111</v>
-      </c>
-      <c r="C53" t="s" s="71">
-        <v>52</v>
-      </c>
-      <c r="D53" s="72">
-        <v>7</v>
-      </c>
-      <c r="E53" s="61"/>
+      <c r="A53" s="70"/>
+      <c r="B53" t="s" s="65">
+        <v>112</v>
+      </c>
+      <c r="C53" t="s" s="66">
+        <v>53</v>
+      </c>
+      <c r="D53" s="67">
+        <v>4</v>
+      </c>
+      <c r="E53" s="45"/>
       <c r="F53" s="30"/>
       <c r="G53" s="30"/>
       <c r="H53" s="30"/>
@@ -7539,17 +7465,17 @@
       <c r="N53" s="30"/>
     </row>
     <row r="54" ht="15.75" customHeight="1">
-      <c r="A54" s="74"/>
-      <c r="B54" t="s" s="67">
-        <v>112</v>
-      </c>
-      <c r="C54" t="s" s="71">
-        <v>53</v>
-      </c>
-      <c r="D54" s="72">
-        <v>4</v>
-      </c>
-      <c r="E54" s="61"/>
+      <c r="A54" s="70"/>
+      <c r="B54" t="s" s="65">
+        <v>113</v>
+      </c>
+      <c r="C54" t="s" s="66">
+        <v>54</v>
+      </c>
+      <c r="D54" s="67">
+        <v>2</v>
+      </c>
+      <c r="E54" s="45"/>
       <c r="F54" s="30"/>
       <c r="G54" s="30"/>
       <c r="H54" s="30"/>
@@ -7561,17 +7487,17 @@
       <c r="N54" s="30"/>
     </row>
     <row r="55" ht="15.75" customHeight="1">
-      <c r="A55" s="74"/>
-      <c r="B55" t="s" s="67">
-        <v>113</v>
-      </c>
-      <c r="C55" t="s" s="71">
-        <v>54</v>
-      </c>
-      <c r="D55" s="72">
-        <v>2</v>
-      </c>
-      <c r="E55" s="61"/>
+      <c r="A55" s="70"/>
+      <c r="B55" t="s" s="65">
+        <v>114</v>
+      </c>
+      <c r="C55" t="s" s="66">
+        <v>55</v>
+      </c>
+      <c r="D55" s="67">
+        <v>6</v>
+      </c>
+      <c r="E55" s="45"/>
       <c r="F55" s="30"/>
       <c r="G55" s="30"/>
       <c r="H55" s="30"/>
@@ -7583,17 +7509,17 @@
       <c r="N55" s="30"/>
     </row>
     <row r="56" ht="15.75" customHeight="1">
-      <c r="A56" s="74"/>
-      <c r="B56" t="s" s="67">
-        <v>114</v>
-      </c>
-      <c r="C56" t="s" s="71">
-        <v>55</v>
-      </c>
-      <c r="D56" s="72">
-        <v>6</v>
-      </c>
-      <c r="E56" s="61"/>
+      <c r="A56" s="70"/>
+      <c r="B56" t="s" s="65">
+        <v>115</v>
+      </c>
+      <c r="C56" t="s" s="66">
+        <v>56</v>
+      </c>
+      <c r="D56" s="67">
+        <v>8</v>
+      </c>
+      <c r="E56" s="45"/>
       <c r="F56" s="30"/>
       <c r="G56" s="30"/>
       <c r="H56" s="30"/>
@@ -7605,17 +7531,17 @@
       <c r="N56" s="30"/>
     </row>
     <row r="57" ht="15.75" customHeight="1">
-      <c r="A57" s="74"/>
-      <c r="B57" t="s" s="67">
-        <v>115</v>
-      </c>
-      <c r="C57" t="s" s="71">
-        <v>56</v>
-      </c>
-      <c r="D57" s="72">
-        <v>8</v>
-      </c>
-      <c r="E57" s="61"/>
+      <c r="A57" s="70"/>
+      <c r="B57" t="s" s="65">
+        <v>116</v>
+      </c>
+      <c r="C57" t="s" s="66">
+        <v>57</v>
+      </c>
+      <c r="D57" s="67">
+        <v>2</v>
+      </c>
+      <c r="E57" s="45"/>
       <c r="F57" s="30"/>
       <c r="G57" s="30"/>
       <c r="H57" s="30"/>
@@ -7627,17 +7553,17 @@
       <c r="N57" s="30"/>
     </row>
     <row r="58" ht="15.75" customHeight="1">
-      <c r="A58" s="74"/>
-      <c r="B58" t="s" s="67">
-        <v>116</v>
-      </c>
-      <c r="C58" t="s" s="71">
-        <v>57</v>
-      </c>
-      <c r="D58" s="72">
+      <c r="A58" s="70"/>
+      <c r="B58" t="s" s="65">
+        <v>117</v>
+      </c>
+      <c r="C58" t="s" s="66">
+        <v>58</v>
+      </c>
+      <c r="D58" s="67">
         <v>2</v>
       </c>
-      <c r="E58" s="61"/>
+      <c r="E58" s="45"/>
       <c r="F58" s="30"/>
       <c r="G58" s="30"/>
       <c r="H58" s="30"/>
@@ -7649,17 +7575,17 @@
       <c r="N58" s="30"/>
     </row>
     <row r="59" ht="15.75" customHeight="1">
-      <c r="A59" s="74"/>
-      <c r="B59" t="s" s="67">
-        <v>117</v>
-      </c>
-      <c r="C59" t="s" s="71">
-        <v>58</v>
-      </c>
-      <c r="D59" s="72">
-        <v>2</v>
-      </c>
-      <c r="E59" s="61"/>
+      <c r="A59" s="70"/>
+      <c r="B59" t="s" s="65">
+        <v>118</v>
+      </c>
+      <c r="C59" t="s" s="66">
+        <v>59</v>
+      </c>
+      <c r="D59" s="67">
+        <v>6</v>
+      </c>
+      <c r="E59" s="45"/>
       <c r="F59" s="30"/>
       <c r="G59" s="30"/>
       <c r="H59" s="30"/>
@@ -7671,17 +7597,17 @@
       <c r="N59" s="30"/>
     </row>
     <row r="60" ht="15.75" customHeight="1">
-      <c r="A60" s="74"/>
-      <c r="B60" t="s" s="67">
-        <v>118</v>
-      </c>
-      <c r="C60" t="s" s="71">
-        <v>59</v>
-      </c>
-      <c r="D60" s="72">
-        <v>6</v>
-      </c>
-      <c r="E60" s="61"/>
+      <c r="A60" s="70"/>
+      <c r="B60" t="s" s="65">
+        <v>119</v>
+      </c>
+      <c r="C60" t="s" s="66">
+        <v>60</v>
+      </c>
+      <c r="D60" s="67">
+        <v>1</v>
+      </c>
+      <c r="E60" s="45"/>
       <c r="F60" s="30"/>
       <c r="G60" s="30"/>
       <c r="H60" s="30"/>
@@ -7693,17 +7619,11 @@
       <c r="N60" s="30"/>
     </row>
     <row r="61" ht="15.75" customHeight="1">
-      <c r="A61" s="74"/>
-      <c r="B61" t="s" s="67">
-        <v>119</v>
-      </c>
-      <c r="C61" t="s" s="71">
-        <v>60</v>
-      </c>
-      <c r="D61" s="72">
-        <v>1</v>
-      </c>
-      <c r="E61" s="61"/>
+      <c r="A61" s="70"/>
+      <c r="B61" s="71"/>
+      <c r="C61" s="30"/>
+      <c r="D61" s="67"/>
+      <c r="E61" s="45"/>
       <c r="F61" s="30"/>
       <c r="G61" s="30"/>
       <c r="H61" s="30"/>
@@ -7715,11 +7635,11 @@
       <c r="N61" s="30"/>
     </row>
     <row r="62" ht="15.75" customHeight="1">
-      <c r="A62" s="74"/>
-      <c r="B62" s="75"/>
+      <c r="A62" s="70"/>
+      <c r="B62" s="45"/>
       <c r="C62" s="30"/>
-      <c r="D62" s="72"/>
-      <c r="E62" s="61"/>
+      <c r="D62" s="67"/>
+      <c r="E62" s="45"/>
       <c r="F62" s="30"/>
       <c r="G62" s="30"/>
       <c r="H62" s="30"/>
@@ -7731,11 +7651,11 @@
       <c r="N62" s="30"/>
     </row>
     <row r="63" ht="15.75" customHeight="1">
-      <c r="A63" s="74"/>
-      <c r="B63" s="76"/>
+      <c r="A63" s="70"/>
+      <c r="B63" s="45"/>
       <c r="C63" s="30"/>
-      <c r="D63" s="72"/>
-      <c r="E63" s="61"/>
+      <c r="D63" s="67"/>
+      <c r="E63" s="45"/>
       <c r="F63" s="30"/>
       <c r="G63" s="30"/>
       <c r="H63" s="30"/>
@@ -7747,11 +7667,11 @@
       <c r="N63" s="30"/>
     </row>
     <row r="64" ht="15.75" customHeight="1">
-      <c r="A64" s="74"/>
-      <c r="B64" s="76"/>
+      <c r="A64" s="70"/>
+      <c r="B64" s="45"/>
       <c r="C64" s="30"/>
-      <c r="D64" s="72"/>
-      <c r="E64" s="61"/>
+      <c r="D64" s="67"/>
+      <c r="E64" s="45"/>
       <c r="F64" s="30"/>
       <c r="G64" s="30"/>
       <c r="H64" s="30"/>
@@ -7763,11 +7683,11 @@
       <c r="N64" s="30"/>
     </row>
     <row r="65" ht="15.75" customHeight="1">
-      <c r="A65" s="74"/>
-      <c r="B65" s="76"/>
+      <c r="A65" s="70"/>
+      <c r="B65" s="45"/>
       <c r="C65" s="30"/>
-      <c r="D65" s="72"/>
-      <c r="E65" s="61"/>
+      <c r="D65" s="67"/>
+      <c r="E65" s="45"/>
       <c r="F65" s="30"/>
       <c r="G65" s="30"/>
       <c r="H65" s="30"/>
@@ -7779,11 +7699,11 @@
       <c r="N65" s="30"/>
     </row>
     <row r="66" ht="15.75" customHeight="1">
-      <c r="A66" s="74"/>
-      <c r="B66" s="76"/>
+      <c r="A66" s="70"/>
+      <c r="B66" s="45"/>
       <c r="C66" s="30"/>
-      <c r="D66" s="72"/>
-      <c r="E66" s="61"/>
+      <c r="D66" s="67"/>
+      <c r="E66" s="45"/>
       <c r="F66" s="30"/>
       <c r="G66" s="30"/>
       <c r="H66" s="30"/>
@@ -7795,11 +7715,11 @@
       <c r="N66" s="30"/>
     </row>
     <row r="67" ht="15.75" customHeight="1">
-      <c r="A67" s="74"/>
-      <c r="B67" s="76"/>
+      <c r="A67" s="70"/>
+      <c r="B67" s="45"/>
       <c r="C67" s="30"/>
-      <c r="D67" s="72"/>
-      <c r="E67" s="61"/>
+      <c r="D67" s="67"/>
+      <c r="E67" s="45"/>
       <c r="F67" s="30"/>
       <c r="G67" s="30"/>
       <c r="H67" s="30"/>
@@ -7811,11 +7731,11 @@
       <c r="N67" s="30"/>
     </row>
     <row r="68" ht="15.75" customHeight="1">
-      <c r="A68" s="74"/>
-      <c r="B68" s="76"/>
+      <c r="A68" s="70"/>
+      <c r="B68" s="45"/>
       <c r="C68" s="30"/>
-      <c r="D68" s="72"/>
-      <c r="E68" s="61"/>
+      <c r="D68" s="67"/>
+      <c r="E68" s="45"/>
       <c r="F68" s="30"/>
       <c r="G68" s="30"/>
       <c r="H68" s="30"/>
@@ -7827,11 +7747,11 @@
       <c r="N68" s="30"/>
     </row>
     <row r="69" ht="15.75" customHeight="1">
-      <c r="A69" s="74"/>
-      <c r="B69" s="76"/>
+      <c r="A69" s="70"/>
+      <c r="B69" s="45"/>
       <c r="C69" s="30"/>
-      <c r="D69" s="72"/>
-      <c r="E69" s="61"/>
+      <c r="D69" s="67"/>
+      <c r="E69" s="45"/>
       <c r="F69" s="30"/>
       <c r="G69" s="30"/>
       <c r="H69" s="30"/>
@@ -7843,11 +7763,11 @@
       <c r="N69" s="30"/>
     </row>
     <row r="70" ht="15.75" customHeight="1">
-      <c r="A70" s="74"/>
-      <c r="B70" s="76"/>
+      <c r="A70" s="70"/>
+      <c r="B70" s="45"/>
       <c r="C70" s="30"/>
-      <c r="D70" s="72"/>
-      <c r="E70" s="61"/>
+      <c r="D70" s="67"/>
+      <c r="E70" s="45"/>
       <c r="F70" s="30"/>
       <c r="G70" s="30"/>
       <c r="H70" s="30"/>
@@ -7859,11 +7779,11 @@
       <c r="N70" s="30"/>
     </row>
     <row r="71" ht="15.75" customHeight="1">
-      <c r="A71" s="74"/>
-      <c r="B71" s="76"/>
+      <c r="A71" s="70"/>
+      <c r="B71" s="45"/>
       <c r="C71" s="30"/>
-      <c r="D71" s="72"/>
-      <c r="E71" s="61"/>
+      <c r="D71" s="67"/>
+      <c r="E71" s="45"/>
       <c r="F71" s="30"/>
       <c r="G71" s="30"/>
       <c r="H71" s="30"/>
@@ -7875,11 +7795,11 @@
       <c r="N71" s="30"/>
     </row>
     <row r="72" ht="15.75" customHeight="1">
-      <c r="A72" s="74"/>
-      <c r="B72" s="76"/>
+      <c r="A72" s="70"/>
+      <c r="B72" s="45"/>
       <c r="C72" s="30"/>
-      <c r="D72" s="72"/>
-      <c r="E72" s="61"/>
+      <c r="D72" s="67"/>
+      <c r="E72" s="45"/>
       <c r="F72" s="30"/>
       <c r="G72" s="30"/>
       <c r="H72" s="30"/>
@@ -7891,11 +7811,11 @@
       <c r="N72" s="30"/>
     </row>
     <row r="73" ht="15.75" customHeight="1">
-      <c r="A73" s="74"/>
-      <c r="B73" s="76"/>
+      <c r="A73" s="70"/>
+      <c r="B73" s="45"/>
       <c r="C73" s="30"/>
-      <c r="D73" s="72"/>
-      <c r="E73" s="61"/>
+      <c r="D73" s="67"/>
+      <c r="E73" s="45"/>
       <c r="F73" s="30"/>
       <c r="G73" s="30"/>
       <c r="H73" s="30"/>
@@ -7907,11 +7827,11 @@
       <c r="N73" s="30"/>
     </row>
     <row r="74" ht="15.75" customHeight="1">
-      <c r="A74" s="74"/>
-      <c r="B74" s="76"/>
+      <c r="A74" s="70"/>
+      <c r="B74" s="45"/>
       <c r="C74" s="30"/>
-      <c r="D74" s="72"/>
-      <c r="E74" s="61"/>
+      <c r="D74" s="67"/>
+      <c r="E74" s="45"/>
       <c r="F74" s="30"/>
       <c r="G74" s="30"/>
       <c r="H74" s="30"/>
@@ -7923,11 +7843,11 @@
       <c r="N74" s="30"/>
     </row>
     <row r="75" ht="15.75" customHeight="1">
-      <c r="A75" s="74"/>
-      <c r="B75" s="76"/>
+      <c r="A75" s="70"/>
+      <c r="B75" s="45"/>
       <c r="C75" s="30"/>
-      <c r="D75" s="72"/>
-      <c r="E75" s="61"/>
+      <c r="D75" s="67"/>
+      <c r="E75" s="45"/>
       <c r="F75" s="30"/>
       <c r="G75" s="30"/>
       <c r="H75" s="30"/>
@@ -7939,11 +7859,11 @@
       <c r="N75" s="30"/>
     </row>
     <row r="76" ht="15.75" customHeight="1">
-      <c r="A76" s="74"/>
-      <c r="B76" s="76"/>
+      <c r="A76" s="70"/>
+      <c r="B76" s="45"/>
       <c r="C76" s="30"/>
-      <c r="D76" s="72"/>
-      <c r="E76" s="61"/>
+      <c r="D76" s="67"/>
+      <c r="E76" s="45"/>
       <c r="F76" s="30"/>
       <c r="G76" s="30"/>
       <c r="H76" s="30"/>
@@ -7955,11 +7875,11 @@
       <c r="N76" s="30"/>
     </row>
     <row r="77" ht="15.75" customHeight="1">
-      <c r="A77" s="74"/>
-      <c r="B77" s="76"/>
+      <c r="A77" s="70"/>
+      <c r="B77" s="45"/>
       <c r="C77" s="30"/>
-      <c r="D77" s="72"/>
-      <c r="E77" s="61"/>
+      <c r="D77" s="67"/>
+      <c r="E77" s="45"/>
       <c r="F77" s="30"/>
       <c r="G77" s="30"/>
       <c r="H77" s="30"/>
@@ -7971,11 +7891,11 @@
       <c r="N77" s="30"/>
     </row>
     <row r="78" ht="15.75" customHeight="1">
-      <c r="A78" s="74"/>
-      <c r="B78" s="76"/>
+      <c r="A78" s="70"/>
+      <c r="B78" s="45"/>
       <c r="C78" s="30"/>
-      <c r="D78" s="72"/>
-      <c r="E78" s="61"/>
+      <c r="D78" s="67"/>
+      <c r="E78" s="45"/>
       <c r="F78" s="30"/>
       <c r="G78" s="30"/>
       <c r="H78" s="30"/>
@@ -7987,11 +7907,11 @@
       <c r="N78" s="30"/>
     </row>
     <row r="79" ht="15.75" customHeight="1">
-      <c r="A79" s="74"/>
-      <c r="B79" s="76"/>
+      <c r="A79" s="70"/>
+      <c r="B79" s="45"/>
       <c r="C79" s="30"/>
-      <c r="D79" s="72"/>
-      <c r="E79" s="61"/>
+      <c r="D79" s="67"/>
+      <c r="E79" s="45"/>
       <c r="F79" s="30"/>
       <c r="G79" s="30"/>
       <c r="H79" s="30"/>
@@ -8003,11 +7923,11 @@
       <c r="N79" s="30"/>
     </row>
     <row r="80" ht="15.75" customHeight="1">
-      <c r="A80" s="74"/>
-      <c r="B80" s="76"/>
+      <c r="A80" s="70"/>
+      <c r="B80" s="45"/>
       <c r="C80" s="30"/>
-      <c r="D80" s="72"/>
-      <c r="E80" s="61"/>
+      <c r="D80" s="67"/>
+      <c r="E80" s="45"/>
       <c r="F80" s="30"/>
       <c r="G80" s="30"/>
       <c r="H80" s="30"/>
@@ -8019,11 +7939,11 @@
       <c r="N80" s="30"/>
     </row>
     <row r="81" ht="15.75" customHeight="1">
-      <c r="A81" s="74"/>
-      <c r="B81" s="76"/>
+      <c r="A81" s="70"/>
+      <c r="B81" s="45"/>
       <c r="C81" s="30"/>
-      <c r="D81" s="72"/>
-      <c r="E81" s="61"/>
+      <c r="D81" s="67"/>
+      <c r="E81" s="45"/>
       <c r="F81" s="30"/>
       <c r="G81" s="30"/>
       <c r="H81" s="30"/>
@@ -8035,11 +7955,11 @@
       <c r="N81" s="30"/>
     </row>
     <row r="82" ht="15.75" customHeight="1">
-      <c r="A82" s="74"/>
-      <c r="B82" s="76"/>
+      <c r="A82" s="70"/>
+      <c r="B82" s="45"/>
       <c r="C82" s="30"/>
-      <c r="D82" s="72"/>
-      <c r="E82" s="61"/>
+      <c r="D82" s="67"/>
+      <c r="E82" s="45"/>
       <c r="F82" s="30"/>
       <c r="G82" s="30"/>
       <c r="H82" s="30"/>
@@ -8051,11 +7971,11 @@
       <c r="N82" s="30"/>
     </row>
     <row r="83" ht="15.75" customHeight="1">
-      <c r="A83" s="74"/>
-      <c r="B83" s="76"/>
+      <c r="A83" s="70"/>
+      <c r="B83" s="45"/>
       <c r="C83" s="30"/>
-      <c r="D83" s="72"/>
-      <c r="E83" s="61"/>
+      <c r="D83" s="67"/>
+      <c r="E83" s="45"/>
       <c r="F83" s="30"/>
       <c r="G83" s="30"/>
       <c r="H83" s="30"/>
@@ -8067,11 +7987,11 @@
       <c r="N83" s="30"/>
     </row>
     <row r="84" ht="15.75" customHeight="1">
-      <c r="A84" s="74"/>
-      <c r="B84" s="76"/>
+      <c r="A84" s="70"/>
+      <c r="B84" s="45"/>
       <c r="C84" s="30"/>
-      <c r="D84" s="72"/>
-      <c r="E84" s="61"/>
+      <c r="D84" s="67"/>
+      <c r="E84" s="45"/>
       <c r="F84" s="30"/>
       <c r="G84" s="30"/>
       <c r="H84" s="30"/>
@@ -8083,11 +8003,11 @@
       <c r="N84" s="30"/>
     </row>
     <row r="85" ht="15.75" customHeight="1">
-      <c r="A85" s="74"/>
-      <c r="B85" s="76"/>
+      <c r="A85" s="70"/>
+      <c r="B85" s="45"/>
       <c r="C85" s="30"/>
-      <c r="D85" s="72"/>
-      <c r="E85" s="61"/>
+      <c r="D85" s="67"/>
+      <c r="E85" s="45"/>
       <c r="F85" s="30"/>
       <c r="G85" s="30"/>
       <c r="H85" s="30"/>
@@ -8099,11 +8019,11 @@
       <c r="N85" s="30"/>
     </row>
     <row r="86" ht="15.75" customHeight="1">
-      <c r="A86" s="74"/>
-      <c r="B86" s="76"/>
+      <c r="A86" s="70"/>
+      <c r="B86" s="45"/>
       <c r="C86" s="30"/>
-      <c r="D86" s="72"/>
-      <c r="E86" s="61"/>
+      <c r="D86" s="67"/>
+      <c r="E86" s="45"/>
       <c r="F86" s="30"/>
       <c r="G86" s="30"/>
       <c r="H86" s="30"/>
@@ -8115,11 +8035,11 @@
       <c r="N86" s="30"/>
     </row>
     <row r="87" ht="15.75" customHeight="1">
-      <c r="A87" s="74"/>
-      <c r="B87" s="76"/>
+      <c r="A87" s="70"/>
+      <c r="B87" s="45"/>
       <c r="C87" s="30"/>
-      <c r="D87" s="72"/>
-      <c r="E87" s="61"/>
+      <c r="D87" s="67"/>
+      <c r="E87" s="45"/>
       <c r="F87" s="30"/>
       <c r="G87" s="30"/>
       <c r="H87" s="30"/>
@@ -8131,11 +8051,11 @@
       <c r="N87" s="30"/>
     </row>
     <row r="88" ht="15.75" customHeight="1">
-      <c r="A88" s="74"/>
-      <c r="B88" s="76"/>
+      <c r="A88" s="70"/>
+      <c r="B88" s="45"/>
       <c r="C88" s="30"/>
-      <c r="D88" s="72"/>
-      <c r="E88" s="61"/>
+      <c r="D88" s="67"/>
+      <c r="E88" s="45"/>
       <c r="F88" s="30"/>
       <c r="G88" s="30"/>
       <c r="H88" s="30"/>
@@ -8147,11 +8067,11 @@
       <c r="N88" s="30"/>
     </row>
     <row r="89" ht="15.75" customHeight="1">
-      <c r="A89" s="74"/>
-      <c r="B89" s="76"/>
+      <c r="A89" s="70"/>
+      <c r="B89" s="45"/>
       <c r="C89" s="30"/>
-      <c r="D89" s="72"/>
-      <c r="E89" s="61"/>
+      <c r="D89" s="67"/>
+      <c r="E89" s="45"/>
       <c r="F89" s="30"/>
       <c r="G89" s="30"/>
       <c r="H89" s="30"/>
@@ -8163,11 +8083,11 @@
       <c r="N89" s="30"/>
     </row>
     <row r="90" ht="15.75" customHeight="1">
-      <c r="A90" s="74"/>
-      <c r="B90" s="76"/>
+      <c r="A90" s="70"/>
+      <c r="B90" s="45"/>
       <c r="C90" s="30"/>
-      <c r="D90" s="72"/>
-      <c r="E90" s="61"/>
+      <c r="D90" s="67"/>
+      <c r="E90" s="45"/>
       <c r="F90" s="30"/>
       <c r="G90" s="30"/>
       <c r="H90" s="30"/>
@@ -8179,11 +8099,11 @@
       <c r="N90" s="30"/>
     </row>
     <row r="91" ht="15.75" customHeight="1">
-      <c r="A91" s="74"/>
-      <c r="B91" s="76"/>
+      <c r="A91" s="70"/>
+      <c r="B91" s="45"/>
       <c r="C91" s="30"/>
-      <c r="D91" s="72"/>
-      <c r="E91" s="61"/>
+      <c r="D91" s="67"/>
+      <c r="E91" s="45"/>
       <c r="F91" s="30"/>
       <c r="G91" s="30"/>
       <c r="H91" s="30"/>
@@ -8195,11 +8115,11 @@
       <c r="N91" s="30"/>
     </row>
     <row r="92" ht="15.75" customHeight="1">
-      <c r="A92" s="74"/>
-      <c r="B92" s="76"/>
+      <c r="A92" s="70"/>
+      <c r="B92" s="45"/>
       <c r="C92" s="30"/>
-      <c r="D92" s="72"/>
-      <c r="E92" s="61"/>
+      <c r="D92" s="67"/>
+      <c r="E92" s="45"/>
       <c r="F92" s="30"/>
       <c r="G92" s="30"/>
       <c r="H92" s="30"/>
@@ -8211,11 +8131,11 @@
       <c r="N92" s="30"/>
     </row>
     <row r="93" ht="15.75" customHeight="1">
-      <c r="A93" s="74"/>
-      <c r="B93" s="76"/>
+      <c r="A93" s="70"/>
+      <c r="B93" s="45"/>
       <c r="C93" s="30"/>
-      <c r="D93" s="72"/>
-      <c r="E93" s="61"/>
+      <c r="D93" s="67"/>
+      <c r="E93" s="45"/>
       <c r="F93" s="30"/>
       <c r="G93" s="30"/>
       <c r="H93" s="30"/>
@@ -8227,11 +8147,11 @@
       <c r="N93" s="30"/>
     </row>
     <row r="94" ht="15.75" customHeight="1">
-      <c r="A94" s="74"/>
-      <c r="B94" s="76"/>
+      <c r="A94" s="70"/>
+      <c r="B94" s="45"/>
       <c r="C94" s="30"/>
-      <c r="D94" s="72"/>
-      <c r="E94" s="61"/>
+      <c r="D94" s="67"/>
+      <c r="E94" s="45"/>
       <c r="F94" s="30"/>
       <c r="G94" s="30"/>
       <c r="H94" s="30"/>
@@ -8243,11 +8163,11 @@
       <c r="N94" s="30"/>
     </row>
     <row r="95" ht="15.75" customHeight="1">
-      <c r="A95" s="74"/>
-      <c r="B95" s="76"/>
+      <c r="A95" s="70"/>
+      <c r="B95" s="45"/>
       <c r="C95" s="30"/>
-      <c r="D95" s="72"/>
-      <c r="E95" s="61"/>
+      <c r="D95" s="67"/>
+      <c r="E95" s="45"/>
       <c r="F95" s="30"/>
       <c r="G95" s="30"/>
       <c r="H95" s="30"/>
@@ -8259,11 +8179,11 @@
       <c r="N95" s="30"/>
     </row>
     <row r="96" ht="15.75" customHeight="1">
-      <c r="A96" s="74"/>
-      <c r="B96" s="76"/>
+      <c r="A96" s="70"/>
+      <c r="B96" s="45"/>
       <c r="C96" s="30"/>
-      <c r="D96" s="72"/>
-      <c r="E96" s="61"/>
+      <c r="D96" s="67"/>
+      <c r="E96" s="45"/>
       <c r="F96" s="30"/>
       <c r="G96" s="30"/>
       <c r="H96" s="30"/>
@@ -8275,11 +8195,11 @@
       <c r="N96" s="30"/>
     </row>
     <row r="97" ht="15.75" customHeight="1">
-      <c r="A97" s="74"/>
-      <c r="B97" s="76"/>
+      <c r="A97" s="70"/>
+      <c r="B97" s="45"/>
       <c r="C97" s="30"/>
-      <c r="D97" s="72"/>
-      <c r="E97" s="61"/>
+      <c r="D97" s="67"/>
+      <c r="E97" s="45"/>
       <c r="F97" s="30"/>
       <c r="G97" s="30"/>
       <c r="H97" s="30"/>
@@ -8291,11 +8211,11 @@
       <c r="N97" s="30"/>
     </row>
     <row r="98" ht="15.75" customHeight="1">
-      <c r="A98" s="74"/>
-      <c r="B98" s="76"/>
+      <c r="A98" s="70"/>
+      <c r="B98" s="45"/>
       <c r="C98" s="30"/>
-      <c r="D98" s="72"/>
-      <c r="E98" s="61"/>
+      <c r="D98" s="67"/>
+      <c r="E98" s="45"/>
       <c r="F98" s="30"/>
       <c r="G98" s="30"/>
       <c r="H98" s="30"/>
@@ -8307,11 +8227,11 @@
       <c r="N98" s="30"/>
     </row>
     <row r="99" ht="15.75" customHeight="1">
-      <c r="A99" s="74"/>
-      <c r="B99" s="76"/>
+      <c r="A99" s="72"/>
+      <c r="B99" s="45"/>
       <c r="C99" s="30"/>
-      <c r="D99" s="72"/>
-      <c r="E99" s="61"/>
+      <c r="D99" s="67"/>
+      <c r="E99" s="45"/>
       <c r="F99" s="30"/>
       <c r="G99" s="30"/>
       <c r="H99" s="30"/>
@@ -8321,22 +8241,6 @@
       <c r="L99" s="30"/>
       <c r="M99" s="30"/>
       <c r="N99" s="30"/>
-    </row>
-    <row r="100" ht="15.75" customHeight="1">
-      <c r="A100" s="77"/>
-      <c r="B100" s="76"/>
-      <c r="C100" s="30"/>
-      <c r="D100" s="72"/>
-      <c r="E100" s="61"/>
-      <c r="F100" s="30"/>
-      <c r="G100" s="30"/>
-      <c r="H100" s="30"/>
-      <c r="I100" s="30"/>
-      <c r="J100" s="30"/>
-      <c r="K100" s="30"/>
-      <c r="L100" s="30"/>
-      <c r="M100" s="30"/>
-      <c r="N100" s="30"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>